<commit_message>
0.0.3: Enable spacifying actionsTree defined outside of Store.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoPiniaClassStructure.xlsx
+++ b/meta/program/BlancoPiniaClassStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoPinia/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A90AFD8-E820-EE47-8611-52E17D783ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3872F3F-24FD-5941-8159-A2AD0AF641E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8260" yWindow="1340" windowWidth="22500" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -438,6 +438,20 @@
   </si>
   <si>
     <t>java.util.List&lt;java.util.List&lt;blanco.pinia.valueobject.BlancoPiniaActionsStructure&gt;&gt;</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>importedActionsTree</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>外部定義された ActionsTree を使う場合は型名を指定します。import 文は「 Vueストア定義・Actions・ヘッダ情報」に記述します。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ガイブテイギ </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">カタメイ </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -975,47 +989,47 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1427,10 +1441,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="E46" sqref="E46:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1625,24 +1639,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="54"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="53"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="48"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="54"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="53"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1684,30 +1698,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="49" t="s">
+      <c r="E25" s="54" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1748,7 +1762,7 @@
     </row>
     <row r="29" spans="1:7" ht="47" customHeight="1">
       <c r="A29" s="38">
-        <f t="shared" ref="A29:A44" si="0">A28+1</f>
+        <f t="shared" ref="A29:A45" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -1758,10 +1772,10 @@
         <v>32</v>
       </c>
       <c r="D29" s="40"/>
-      <c r="E29" s="58" t="s">
+      <c r="E29" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="59"/>
+      <c r="F29" s="58"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="47" customHeight="1">
@@ -1776,10 +1790,10 @@
         <v>32</v>
       </c>
       <c r="D30" s="40"/>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="59"/>
+      <c r="F30" s="58"/>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:7" ht="15">
@@ -1814,10 +1828,10 @@
       <c r="D32" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="51"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="15">
@@ -1834,10 +1848,10 @@
       <c r="D33" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="57"/>
+      <c r="F33" s="56"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -1854,10 +1868,10 @@
       <c r="D34" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="56" t="s">
+      <c r="E34" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="F34" s="57"/>
+      <c r="F34" s="56"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1874,10 +1888,10 @@
       <c r="D35" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="56" t="s">
+      <c r="E35" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="57"/>
+      <c r="F35" s="56"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -1894,10 +1908,10 @@
       <c r="D36" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="56" t="s">
+      <c r="E36" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="F36" s="57"/>
+      <c r="F36" s="56"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1914,10 +1928,10 @@
       <c r="D37" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="E37" s="52" t="s">
+      <c r="E37" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="53"/>
+      <c r="F37" s="51"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -1934,10 +1948,10 @@
       <c r="D38" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="E38" s="52" t="s">
+      <c r="E38" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="53"/>
+      <c r="F38" s="51"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -1954,10 +1968,10 @@
       <c r="D39" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="E39" s="52" t="s">
+      <c r="E39" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="F39" s="53"/>
+      <c r="F39" s="51"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
@@ -1972,10 +1986,10 @@
         <v>32</v>
       </c>
       <c r="D40" s="40"/>
-      <c r="E40" s="52" t="s">
+      <c r="E40" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="53"/>
+      <c r="F40" s="51"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="45" customHeight="1">
@@ -1992,10 +2006,10 @@
       <c r="D41" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="52" t="s">
+      <c r="E41" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="55"/>
+      <c r="F41" s="52"/>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7" ht="30">
@@ -2012,10 +2026,10 @@
       <c r="D42" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E42" s="52" t="s">
+      <c r="E42" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="55"/>
+      <c r="F42" s="52"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" ht="30">
@@ -2032,10 +2046,10 @@
       <c r="D43" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="52" t="s">
+      <c r="E43" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="F43" s="55"/>
+      <c r="F43" s="52"/>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" ht="15">
@@ -2050,37 +2064,46 @@
         <v>48</v>
       </c>
       <c r="D44" s="40"/>
-      <c r="E44" s="52" t="s">
+      <c r="E44" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="55"/>
+      <c r="F44" s="52"/>
       <c r="G44"/>
     </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="38"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="40"/>
+    <row r="45" spans="1:7" ht="15">
+      <c r="A45" s="38">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="40" t="s">
+        <v>48</v>
+      </c>
       <c r="D45" s="40"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="55"/>
+      <c r="E45" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="52"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="38"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="53"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="52"/>
       <c r="G46"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="38"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="43"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="51"/>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7">
@@ -2106,8 +2129,8 @@
       <c r="B50" s="39"/>
       <c r="C50" s="40"/>
       <c r="D50" s="40"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="53"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="43"/>
       <c r="G50"/>
     </row>
     <row r="51" spans="1:7">
@@ -2115,36 +2138,41 @@
       <c r="B51" s="39"/>
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
-      <c r="E51" s="52"/>
-      <c r="F51" s="53"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="51"/>
       <c r="G51"/>
     </row>
-    <row r="52" spans="1:7" ht="14" customHeight="1">
-      <c r="A52" s="21"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="60"/>
-      <c r="F52" s="61"/>
+    <row r="52" spans="1:7">
+      <c r="A52" s="38"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="51"/>
       <c r="G52"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" ht="14" customHeight="1">
+      <c r="A53" s="21"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="49"/>
       <c r="G53"/>
     </row>
+    <row r="54" spans="1:7">
+      <c r="G54"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
+  <mergeCells count="31">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
@@ -2155,18 +2183,23 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E44:F44"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D66" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D67" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>